<commit_message>
Cambios en la tarea y mapeos de la transacción
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/tarjetacredito/TarjetaCreditoPropia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/tarjetacredito/TarjetaCreditoPropia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\tarjetacredito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9691F288-9D01-4C8F-8DAF-0649E47DA0B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FBE3FF-57BB-413C-9AD2-5A79BBA03FEC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -143,6 +143,33 @@
   </si>
   <si>
     <t>Ahorros</t>
+  </si>
+  <si>
+    <t>Otro valor</t>
+  </si>
+  <si>
+    <t>*7826</t>
+  </si>
+  <si>
+    <t>Pesos</t>
+  </si>
+  <si>
+    <t>500000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Personal Visa</t>
+  </si>
+  <si>
+    <t>*5880</t>
+  </si>
+  <si>
+    <t>480369</t>
   </si>
 </sst>
 </file>
@@ -569,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -721,14 +748,143 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="O3" s="6"/>
+      <c r="A3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{67C6CB3E-A984-46BB-B622-F0ADD216DE02}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{BBE34ADD-6B07-4872-AD38-7133AF9FBFD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>